<commit_message>
Support average age calculations for UCOD_LONGTERM_COMPARABLE_LEADING
</commit_message>
<xml_diff>
--- a/data/ucod/united_states/comparable_ucod_estimates.xlsx
+++ b/data/ucod/united_states/comparable_ucod_estimates.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="184">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -362,9 +362,6 @@
   </si>
   <si>
     <t xml:space="preserve">V02-V04,V09.0,V09.2,V12-V14,V19.0-V19.2,V19.4-V19.6,V20-V79,V80.3-V80.5,V81.0-V81.1,V82.0-V82.1,V83-V86,V87.0-V87.8,V88.0-V88.8,V89.0,V89.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accidents excluding motor-vehicle</t>
   </si>
   <si>
     <t xml:space="preserve">169,171-195</t>
@@ -8852,7 +8849,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9416,40 +9413,40 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="C15" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>38</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15" s="6" t="n">
         <v>0.925</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I15" s="6" t="n">
         <v>0.9841</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K15" s="6" t="n">
         <v>1.0253</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M15" s="10"/>
     </row>
@@ -9464,23 +9461,23 @@
         <v>0.98</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K16" s="17"/>
       <c r="L16" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9494,27 +9491,27 @@
         <v>0.98</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" s="17" t="n">
         <v>0.92</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I17" s="17" t="n">
         <v>0.9167</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9528,27 +9525,27 @@
         <v>0.99</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" s="17" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I18" s="6" t="n">
         <v>0.8571</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K18" s="17"/>
       <c r="L18" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9556,29 +9553,29 @@
         <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>0.97</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E19" s="6" t="n">
         <v>0.88</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9586,37 +9583,37 @@
         <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>1.06</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E20" s="6" t="n">
         <v>0.97</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G20" s="6" t="n">
         <v>1.185</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I20" s="6" t="n">
         <v>0.1821</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K20" s="6" t="n">
         <v>0.8596</v>
       </c>
       <c r="L20" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9624,34 +9621,34 @@
         <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>1.02</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E21" s="6" t="n">
         <v>0.99</v>
       </c>
       <c r="F21" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="I21" s="6" t="n">
         <v>0.9788</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K21" s="6" t="n">
         <v>0.9896</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9659,31 +9656,31 @@
         <v>23</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>0.99</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E22" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="I22" s="6" t="n">
         <v>0.5</v>
       </c>
       <c r="J22" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9691,37 +9688,37 @@
         <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C23" s="6" t="n">
         <v>0.72</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23" s="6" t="n">
         <v>1.03</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>0.322</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I23" s="6" t="n">
         <v>1.0089</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K23" s="6" t="n">
         <v>0.7808</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9729,31 +9726,31 @@
         <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>2.78</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E24" s="6" t="n">
         <v>0.92</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H24" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>154</v>
-      </c>
       <c r="J24" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K24" s="6" t="n">
         <v>0.4386</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9761,37 +9758,37 @@
         <v>26</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" s="6" t="n">
         <v>6.54</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E25" s="6" t="n">
         <v>1.33</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G25" s="6" t="n">
         <v>0.82</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I25" s="6" t="n">
         <v>1.2703</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K25" s="6" t="n">
         <v>1.1162</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9799,28 +9796,28 @@
         <v>27</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G26" s="6" t="n">
         <v>1.0034</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I26" s="6" t="n">
         <v>1.8846</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K26" s="6" t="n">
         <v>1.0411</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9828,37 +9825,37 @@
         <v>28</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" s="6" t="n">
         <v>0.84</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E27" s="6" t="n">
         <v>1.01</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G27" s="6" t="n">
         <v>0.9856</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I27" s="6" t="n">
         <v>1.1192</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K27" s="6" t="n">
         <v>0.9819</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9866,37 +9863,37 @@
         <v>29</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E28" s="6" t="n">
         <v>1.03</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G28" s="6" t="n">
         <v>0.9472</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I28" s="6" t="n">
         <v>1.0032</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K28" s="6" t="n">
         <v>1.0022</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9904,37 +9901,37 @@
         <v>30</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E29" s="6" t="n">
         <v>1</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G29" s="6" t="n">
         <v>0.9969</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I29" s="6" t="n">
         <v>1.0057</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K29" s="6" t="n">
         <v>1.0009</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -9968,10 +9965,10 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9979,10 +9976,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9990,7 +9987,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9998,7 +9995,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10006,12 +10003,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" s="10"/>
     </row>

</xml_diff>

<commit_message>
Convert manual ICD ranges to queries
</commit_message>
<xml_diff>
--- a/data/ucod/united_states/comparable_ucod_estimates.xlsx
+++ b/data/ucod/united_states/comparable_ucod_estimates.xlsx
@@ -617,9 +617,9 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -765,7 +765,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -3225,7 +3225,7 @@
         <v>19317</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="n">
         <v>1959</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>7780</v>
       </c>
       <c r="G60" s="0" t="n">
-        <v>641342</v>
+        <v>642132</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>191666</v>
@@ -3320,7 +3320,7 @@
         <v>8177</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="n">
         <v>1960</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>7932</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>660981</v>
+        <v>661712</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>193588</v>
@@ -3415,7 +3415,7 @@
         <v>8464</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="n">
         <v>1961</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>7820</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>662788</v>
+        <v>663391</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>192951</v>
@@ -3510,7 +3510,7 @@
         <v>8578</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="n">
         <v>1962</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>8194</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>687462</v>
+        <v>688009</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>197451</v>
@@ -3605,7 +3605,7 @@
         <v>9013</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="n">
         <v>1963</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>8246</v>
       </c>
       <c r="G64" s="0" t="n">
-        <v>707285</v>
+        <v>707830</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>201166</v>
@@ -3700,7 +3700,7 @@
         <v>9225</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="n">
         <v>1964</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>8178</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>699357</v>
+        <v>699861</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>198209</v>
@@ -3795,7 +3795,7 @@
         <v>9814</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="n">
         <v>1965</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>7899</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>711607</v>
+        <v>712087</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>201057</v>
@@ -3890,7 +3890,7 @@
         <v>10712</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="n">
         <v>1966</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>7552</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>726551</v>
+        <v>727002</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>204841</v>
@@ -3985,7 +3985,7 @@
         <v>11606</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="n">
         <v>1967</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>7504</v>
       </c>
       <c r="G68" s="0" t="n">
-        <v>720896</v>
+        <v>721268</v>
       </c>
       <c r="H68" s="0" t="n">
         <v>202184</v>
@@ -4080,7 +4080,7 @@
         <v>13425</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="n">
         <v>1968</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>33568</v>
       </c>
       <c r="P69" s="0" t="n">
-        <v>12267</v>
+        <v>16793</v>
       </c>
       <c r="Q69" s="0" t="n">
         <v>29183</v>
@@ -4175,7 +4175,7 @@
         <v>14686</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="n">
         <v>1969</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>33063</v>
       </c>
       <c r="P70" s="0" t="n">
-        <v>12423</v>
+        <v>17008</v>
       </c>
       <c r="Q70" s="0" t="n">
         <v>29866</v>
@@ -4270,7 +4270,7 @@
         <v>15477</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="n">
         <v>1970</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>31689</v>
       </c>
       <c r="P71" s="0" t="n">
-        <v>12308</v>
+        <v>16879</v>
       </c>
       <c r="Q71" s="0" t="n">
         <v>31421</v>
@@ -4365,7 +4365,7 @@
         <v>16883</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="n">
         <v>1971</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>31530</v>
       </c>
       <c r="P72" s="0" t="n">
-        <v>11643</v>
+        <v>16007</v>
       </c>
       <c r="Q72" s="0" t="n">
         <v>31837</v>
@@ -4460,7 +4460,7 @@
         <v>18816</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="n">
         <v>1972</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>32498</v>
       </c>
       <c r="P73" s="0" t="n">
-        <v>10818</v>
+        <v>14756</v>
       </c>
       <c r="Q73" s="0" t="n">
         <v>32604</v>
@@ -4555,7 +4555,7 @@
         <v>19676</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="n">
         <v>1973</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>32628</v>
       </c>
       <c r="P74" s="0" t="n">
-        <v>10465</v>
+        <v>14122</v>
       </c>
       <c r="Q74" s="0" t="n">
         <v>33377</v>
@@ -4650,7 +4650,7 @@
         <v>20500</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="n">
         <v>1974</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>32243</v>
       </c>
       <c r="P75" s="0" t="n">
-        <v>10172</v>
+        <v>13606</v>
       </c>
       <c r="Q75" s="0" t="n">
         <v>33345</v>
@@ -4745,7 +4745,7 @@
         <v>21513</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="n">
         <v>1975</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>28894</v>
       </c>
       <c r="P76" s="0" t="n">
-        <v>9960</v>
+        <v>13332</v>
       </c>
       <c r="Q76" s="0" t="n">
         <v>31655</v>
@@ -4840,7 +4840,7 @@
         <v>21350</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="n">
         <v>1976</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>29377</v>
       </c>
       <c r="P77" s="0" t="n">
-        <v>9655</v>
+        <v>13075</v>
       </c>
       <c r="Q77" s="0" t="n">
         <v>31478</v>
@@ -4935,7 +4935,7 @@
         <v>19587</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="n">
         <v>1977</v>
       </c>
@@ -4982,7 +4982,7 @@
         <v>28758</v>
       </c>
       <c r="P78" s="0" t="n">
-        <v>9646</v>
+        <v>13051</v>
       </c>
       <c r="Q78" s="0" t="n">
         <v>30879</v>
@@ -5030,7 +5030,7 @@
         <v>20015</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="n">
         <v>1978</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>28951</v>
       </c>
       <c r="P79" s="0" t="n">
-        <v>9586</v>
+        <v>13046</v>
       </c>
       <c r="Q79" s="0" t="n">
         <v>30105</v>
@@ -5125,7 +5125,7 @@
         <v>20498</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="n">
         <v>1979</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>28815</v>
       </c>
       <c r="P80" s="0" t="n">
-        <v>9395</v>
+        <v>13619</v>
       </c>
       <c r="Q80" s="0" t="n">
         <v>29759</v>
@@ -5220,7 +5220,7 @@
         <v>22625</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="n">
         <v>1980</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>29457</v>
       </c>
       <c r="P81" s="0" t="n">
-        <v>9664</v>
+        <v>14010</v>
       </c>
       <c r="Q81" s="0" t="n">
         <v>30630</v>
@@ -5315,7 +5315,7 @@
         <v>24363</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="n">
         <v>1981</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>27861</v>
       </c>
       <c r="P82" s="0" t="n">
-        <v>9228</v>
+        <v>13511</v>
       </c>
       <c r="Q82" s="0" t="n">
         <v>29185</v>
@@ -5410,7 +5410,7 @@
         <v>23619</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="n">
         <v>1982</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>26856</v>
       </c>
       <c r="P83" s="0" t="n">
-        <v>9390</v>
+        <v>13670</v>
       </c>
       <c r="Q83" s="0" t="n">
         <v>27658</v>
@@ -5505,7 +5505,7 @@
         <v>22546</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="n">
         <v>1983</v>
       </c>
@@ -5552,7 +5552,7 @@
         <v>26378</v>
       </c>
       <c r="P84" s="0" t="n">
-        <v>9103</v>
+        <v>13258</v>
       </c>
       <c r="Q84" s="0" t="n">
         <v>27302</v>
@@ -5600,7 +5600,7 @@
         <v>20265</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="n">
         <v>1984</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>24470</v>
       </c>
       <c r="P85" s="0" t="n">
-        <v>8884</v>
+        <v>13104</v>
       </c>
       <c r="Q85" s="0" t="n">
         <v>27362</v>
@@ -5695,7 +5695,7 @@
         <v>19870</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="n">
         <v>1985</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>23931</v>
       </c>
       <c r="P86" s="0" t="n">
-        <v>8741</v>
+        <v>12863</v>
       </c>
       <c r="Q86" s="0" t="n">
         <v>26812</v>
@@ -5790,7 +5790,7 @@
         <v>19981</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="n">
         <v>1986</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>22720</v>
       </c>
       <c r="P87" s="0" t="n">
-        <v>8571</v>
+        <v>12708</v>
       </c>
       <c r="Q87" s="0" t="n">
         <v>26194</v>
@@ -5885,7 +5885,7 @@
         <v>21827</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="n">
         <v>1987</v>
       </c>
@@ -5932,7 +5932,7 @@
         <v>22480</v>
       </c>
       <c r="P88" s="0" t="n">
-        <v>8525</v>
+        <v>12386</v>
       </c>
       <c r="Q88" s="0" t="n">
         <v>26239</v>
@@ -5980,7 +5980,7 @@
         <v>21189</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="n">
         <v>1988</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>22092</v>
       </c>
       <c r="P89" s="0" t="n">
-        <v>8796</v>
+        <v>12824</v>
       </c>
       <c r="Q89" s="0" t="n">
         <v>26461</v>
@@ -6075,7 +6075,7 @@
         <v>22129</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="n">
         <v>1989</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>19372</v>
       </c>
       <c r="P90" s="0" t="n">
-        <v>8876</v>
+        <v>12963</v>
       </c>
       <c r="Q90" s="0" t="n">
         <v>26729</v>
@@ -6170,7 +6170,7 @@
         <v>22993</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="n">
         <v>1990</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>18056</v>
       </c>
       <c r="P91" s="0" t="n">
-        <v>8949</v>
+        <v>13165</v>
       </c>
       <c r="Q91" s="0" t="n">
         <v>25856</v>
@@ -6265,7 +6265,7 @@
         <v>25020</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="n">
         <v>1991</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>17432</v>
       </c>
       <c r="P92" s="0" t="n">
-        <v>8534</v>
+        <v>12674</v>
       </c>
       <c r="Q92" s="0" t="n">
         <v>25473</v>
@@ -6360,7 +6360,7 @@
         <v>26616</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="n">
         <v>1992</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>16836</v>
       </c>
       <c r="P93" s="0" t="n">
-        <v>8555</v>
+        <v>12565</v>
       </c>
       <c r="Q93" s="0" t="n">
         <v>25306</v>
@@ -6455,7 +6455,7 @@
         <v>25577</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="n">
         <v>1993</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>17282</v>
       </c>
       <c r="P94" s="0" t="n">
-        <v>8409</v>
+        <v>12507</v>
       </c>
       <c r="Q94" s="0" t="n">
         <v>25246</v>
@@ -6550,7 +6550,7 @@
         <v>26084</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="n">
         <v>1994</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>17124</v>
       </c>
       <c r="P95" s="0" t="n">
-        <v>8228</v>
+        <v>12092</v>
       </c>
       <c r="Q95" s="0" t="n">
         <v>25447</v>
@@ -6645,7 +6645,7 @@
         <v>25017</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="n">
         <v>1995</v>
       </c>
@@ -6692,7 +6692,7 @@
         <v>16727</v>
       </c>
       <c r="P96" s="0" t="n">
-        <v>8087</v>
+        <v>11949</v>
       </c>
       <c r="Q96" s="0" t="n">
         <v>25262</v>
@@ -6740,7 +6740,7 @@
         <v>22981</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="n">
         <v>1996</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>16749</v>
       </c>
       <c r="P97" s="0" t="n">
-        <v>8138</v>
+        <v>11889</v>
       </c>
       <c r="Q97" s="0" t="n">
         <v>25084</v>
@@ -6835,7 +6835,7 @@
         <v>21058</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="n">
         <v>1997</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>16059</v>
       </c>
       <c r="P98" s="0" t="n">
-        <v>8157</v>
+        <v>11961</v>
       </c>
       <c r="Q98" s="0" t="n">
         <v>25215</v>
@@ -6930,7 +6930,7 @@
         <v>19914</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="n">
         <v>1998</v>
       </c>
@@ -6977,7 +6977,7 @@
         <v>15287</v>
       </c>
       <c r="P99" s="0" t="n">
-        <v>8125</v>
+        <v>11987</v>
       </c>
       <c r="Q99" s="0" t="n">
         <v>25236</v>
@@ -7025,7 +7025,7 @@
         <v>18325</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="n">
         <v>1999</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>35554</v>
       </c>
       <c r="J100" s="0" t="n">
-        <v>73555</v>
+        <v>55755</v>
       </c>
       <c r="K100" s="0" t="n">
         <v>550373</v>
@@ -7066,7 +7066,7 @@
         <v>68462</v>
       </c>
       <c r="N100" s="0" t="n">
-        <v>44408</v>
+        <v>42733</v>
       </c>
       <c r="O100" s="0" t="n">
         <v>14985</v>
@@ -7078,7 +7078,7 @@
         <v>26298</v>
       </c>
       <c r="R100" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S100" s="0" t="n">
         <v>2</v>
@@ -7105,7 +7105,7 @@
         <v>30</v>
       </c>
       <c r="AA100" s="0" t="n">
-        <v>39750</v>
+        <v>16974</v>
       </c>
       <c r="AB100" s="0" t="n">
         <v>124274</v>
@@ -7114,13 +7114,13 @@
         <v>4611</v>
       </c>
       <c r="AD100" s="0" t="n">
-        <v>31330</v>
+        <v>29260</v>
       </c>
       <c r="AE100" s="0" t="n">
-        <v>19311</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17353</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="n">
         <v>2000</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>37284</v>
       </c>
       <c r="J101" s="0" t="n">
-        <v>73001</v>
+        <v>54912</v>
       </c>
       <c r="K101" s="0" t="n">
         <v>553679</v>
@@ -7161,7 +7161,7 @@
         <v>69366</v>
       </c>
       <c r="N101" s="0" t="n">
-        <v>44765</v>
+        <v>43710</v>
       </c>
       <c r="O101" s="0" t="n">
         <v>14396</v>
@@ -7173,7 +7173,7 @@
         <v>26602</v>
       </c>
       <c r="R101" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S101" s="0" t="n">
         <v>1</v>
@@ -7200,7 +7200,7 @@
         <v>37</v>
       </c>
       <c r="AA101" s="0" t="n">
-        <v>41923</v>
+        <v>18087</v>
       </c>
       <c r="AB101" s="0" t="n">
         <v>122118</v>
@@ -7209,13 +7209,13 @@
         <v>4565</v>
       </c>
       <c r="AD101" s="0" t="n">
-        <v>31474</v>
+        <v>29416</v>
       </c>
       <c r="AE101" s="0" t="n">
-        <v>19113</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17191</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="n">
         <v>2001</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>39511</v>
       </c>
       <c r="J102" s="0" t="n">
-        <v>75666</v>
+        <v>58134</v>
       </c>
       <c r="K102" s="0" t="n">
         <v>554371</v>
@@ -7256,7 +7256,7 @@
         <v>71439</v>
       </c>
       <c r="N102" s="0" t="n">
-        <v>44980</v>
+        <v>44091</v>
       </c>
       <c r="O102" s="0" t="n">
         <v>14092</v>
@@ -7295,7 +7295,7 @@
         <v>65</v>
       </c>
       <c r="AA102" s="0" t="n">
-        <v>44028</v>
+        <v>19260</v>
       </c>
       <c r="AB102" s="0" t="n">
         <v>123105</v>
@@ -7304,13 +7304,13 @@
         <v>4498</v>
       </c>
       <c r="AD102" s="0" t="n">
-        <v>32973</v>
+        <v>30672</v>
       </c>
       <c r="AE102" s="0" t="n">
-        <v>20007</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17838</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="n">
         <v>2002</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>41009</v>
       </c>
       <c r="J103" s="0" t="n">
-        <v>78679</v>
+        <v>61751</v>
       </c>
       <c r="K103" s="0" t="n">
         <v>557821</v>
@@ -7351,7 +7351,7 @@
         <v>73315</v>
       </c>
       <c r="N103" s="0" t="n">
-        <v>46263</v>
+        <v>45720</v>
       </c>
       <c r="O103" s="0" t="n">
         <v>13827</v>
@@ -7390,7 +7390,7 @@
         <v>53</v>
       </c>
       <c r="AA103" s="0" t="n">
-        <v>46906</v>
+        <v>20270</v>
       </c>
       <c r="AB103" s="0" t="n">
         <v>124906</v>
@@ -7399,13 +7399,13 @@
         <v>4084</v>
       </c>
       <c r="AD103" s="0" t="n">
-        <v>34063</v>
+        <v>31700</v>
       </c>
       <c r="AE103" s="0" t="n">
-        <v>20322</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18089</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="n">
         <v>2003</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>42497</v>
       </c>
       <c r="J104" s="0" t="n">
-        <v>81553</v>
+        <v>64940</v>
       </c>
       <c r="K104" s="0" t="n">
         <v>557531</v>
@@ -7446,7 +7446,7 @@
         <v>74289</v>
       </c>
       <c r="N104" s="0" t="n">
-        <v>46008</v>
+        <v>45104</v>
       </c>
       <c r="O104" s="0" t="n">
         <v>13057</v>
@@ -7485,7 +7485,7 @@
         <v>41</v>
       </c>
       <c r="AA104" s="0" t="n">
-        <v>50386</v>
+        <v>21956</v>
       </c>
       <c r="AB104" s="0" t="n">
         <v>126480</v>
@@ -7494,13 +7494,13 @@
         <v>3920</v>
       </c>
       <c r="AD104" s="0" t="n">
-        <v>33917</v>
+        <v>31531</v>
       </c>
       <c r="AE104" s="0" t="n">
-        <v>20474</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18246</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="n">
         <v>2004</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>42512</v>
       </c>
       <c r="J105" s="0" t="n">
-        <v>84910</v>
+        <v>67477</v>
       </c>
       <c r="K105" s="0" t="n">
         <v>554470</v>
@@ -7541,7 +7541,7 @@
         <v>73221</v>
       </c>
       <c r="N105" s="0" t="n">
-        <v>46003</v>
+        <v>45277</v>
       </c>
       <c r="O105" s="0" t="n">
         <v>11864</v>
@@ -7580,7 +7580,7 @@
         <v>33</v>
       </c>
       <c r="AA105" s="0" t="n">
-        <v>51762</v>
+        <v>23095</v>
       </c>
       <c r="AB105" s="0" t="n">
         <v>122096</v>
@@ -7589,13 +7589,13 @@
         <v>3692</v>
       </c>
       <c r="AD105" s="0" t="n">
-        <v>34892</v>
+        <v>32488</v>
       </c>
       <c r="AE105" s="0" t="n">
-        <v>20112</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17829</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="n">
         <v>2005</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>43944</v>
       </c>
       <c r="J106" s="0" t="n">
-        <v>91216</v>
+        <v>73029</v>
       </c>
       <c r="K106" s="0" t="n">
         <v>559962</v>
@@ -7636,7 +7636,7 @@
         <v>75207</v>
       </c>
       <c r="N106" s="0" t="n">
-        <v>46423</v>
+        <v>45711</v>
       </c>
       <c r="O106" s="0" t="n">
         <v>11848</v>
@@ -7675,7 +7675,7 @@
         <v>29</v>
       </c>
       <c r="AA106" s="0" t="n">
-        <v>54289</v>
+        <v>24926</v>
       </c>
       <c r="AB106" s="0" t="n">
         <v>131060</v>
@@ -7684,13 +7684,13 @@
         <v>3488</v>
       </c>
       <c r="AD106" s="0" t="n">
-        <v>35183</v>
+        <v>32708</v>
       </c>
       <c r="AE106" s="0" t="n">
-        <v>20945</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18632</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="n">
         <v>2006</v>
       </c>
@@ -7719,7 +7719,7 @@
         <v>45386</v>
       </c>
       <c r="J107" s="0" t="n">
-        <v>95553</v>
+        <v>76806</v>
       </c>
       <c r="K107" s="0" t="n">
         <v>560537</v>
@@ -7731,7 +7731,7 @@
         <v>72525</v>
       </c>
       <c r="N107" s="0" t="n">
-        <v>46297</v>
+        <v>45694</v>
       </c>
       <c r="O107" s="0" t="n">
         <v>8660</v>
@@ -7770,7 +7770,7 @@
         <v>25</v>
       </c>
       <c r="AA107" s="0" t="n">
-        <v>53734</v>
+        <v>23858</v>
       </c>
       <c r="AB107" s="0" t="n">
         <v>124724</v>
@@ -7779,13 +7779,13 @@
         <v>3338</v>
       </c>
       <c r="AD107" s="0" t="n">
-        <v>35915</v>
+        <v>33400</v>
       </c>
       <c r="AE107" s="0" t="n">
-        <v>21473</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19117</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="n">
         <v>2007</v>
       </c>
@@ -7814,7 +7814,7 @@
         <v>46495</v>
       </c>
       <c r="J108" s="0" t="n">
-        <v>99400</v>
+        <v>80273</v>
       </c>
       <c r="K108" s="0" t="n">
         <v>563569</v>
@@ -7826,7 +7826,7 @@
         <v>71459</v>
       </c>
       <c r="N108" s="0" t="n">
-        <v>44852</v>
+        <v>44299</v>
       </c>
       <c r="O108" s="0" t="n">
         <v>8239</v>
@@ -7838,7 +7838,7 @@
         <v>29253</v>
       </c>
       <c r="R108" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S108" s="0" t="n">
         <v>0</v>
@@ -7865,7 +7865,7 @@
         <v>32</v>
       </c>
       <c r="AA108" s="0" t="n">
-        <v>54862</v>
+        <v>23980</v>
       </c>
       <c r="AB108" s="0" t="n">
         <v>128076</v>
@@ -7874,13 +7874,13 @@
         <v>3055</v>
       </c>
       <c r="AD108" s="0" t="n">
-        <v>37346</v>
+        <v>34691</v>
       </c>
       <c r="AE108" s="0" t="n">
-        <v>21388</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18903</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="n">
         <v>2008</v>
       </c>
@@ -7909,7 +7909,7 @@
         <v>48277</v>
       </c>
       <c r="J109" s="0" t="n">
-        <v>100876</v>
+        <v>82654</v>
       </c>
       <c r="K109" s="0" t="n">
         <v>566215</v>
@@ -7921,7 +7921,7 @@
         <v>70649</v>
       </c>
       <c r="N109" s="0" t="n">
-        <v>40677</v>
+        <v>40129</v>
       </c>
       <c r="O109" s="0" t="n">
         <v>7836</v>
@@ -7960,7 +7960,7 @@
         <v>28</v>
       </c>
       <c r="AA109" s="0" t="n">
-        <v>58282</v>
+        <v>25767</v>
       </c>
       <c r="AB109" s="0" t="n">
         <v>141246</v>
@@ -7969,13 +7969,13 @@
         <v>3083</v>
       </c>
       <c r="AD109" s="0" t="n">
-        <v>38850</v>
+        <v>36132</v>
       </c>
       <c r="AE109" s="0" t="n">
-        <v>20844</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18309</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="n">
         <v>2009</v>
       </c>
@@ -8004,7 +8004,7 @@
         <v>48959</v>
       </c>
       <c r="J110" s="0" t="n">
-        <v>99171</v>
+        <v>82319</v>
       </c>
       <c r="K110" s="0" t="n">
         <v>568226</v>
@@ -8016,7 +8016,7 @@
         <v>68776</v>
       </c>
       <c r="N110" s="0" t="n">
-        <v>36993</v>
+        <v>36473</v>
       </c>
       <c r="O110" s="0" t="n">
         <v>7380</v>
@@ -8028,7 +8028,7 @@
         <v>30627</v>
       </c>
       <c r="R110" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S110" s="0" t="n">
         <v>2</v>
@@ -8055,7 +8055,7 @@
         <v>39</v>
       </c>
       <c r="AA110" s="0" t="n">
-        <v>59009</v>
+        <v>25755</v>
       </c>
       <c r="AB110" s="0" t="n">
         <v>137473</v>
@@ -8064,13 +8064,13 @@
         <v>2965</v>
       </c>
       <c r="AD110" s="0" t="n">
-        <v>39577</v>
+        <v>37006</v>
       </c>
       <c r="AE110" s="0" t="n">
-        <v>19677</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17285</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="n">
         <v>2010</v>
       </c>
@@ -8099,7 +8099,7 @@
         <v>50508</v>
       </c>
       <c r="J111" s="0" t="n">
-        <v>104396</v>
+        <v>86043</v>
       </c>
       <c r="K111" s="0" t="n">
         <v>575388</v>
@@ -8111,7 +8111,7 @@
         <v>69154</v>
       </c>
       <c r="N111" s="0" t="n">
-        <v>36020</v>
+        <v>35590</v>
       </c>
       <c r="O111" s="0" t="n">
         <v>7233</v>
@@ -8150,7 +8150,7 @@
         <v>29</v>
       </c>
       <c r="AA111" s="0" t="n">
-        <v>60449</v>
+        <v>26652</v>
       </c>
       <c r="AB111" s="0" t="n">
         <v>138224</v>
@@ -8159,13 +8159,13 @@
         <v>2983</v>
       </c>
       <c r="AD111" s="0" t="n">
-        <v>40905</v>
+        <v>38441</v>
       </c>
       <c r="AE111" s="0" t="n">
-        <v>18995</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16726</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="n">
         <v>2011</v>
       </c>
@@ -8194,7 +8194,7 @@
         <v>45635</v>
       </c>
       <c r="J112" s="0" t="n">
-        <v>109102</v>
+        <v>91666</v>
       </c>
       <c r="K112" s="0" t="n">
         <v>577320</v>
@@ -8206,7 +8206,7 @@
         <v>73916</v>
       </c>
       <c r="N112" s="0" t="n">
-        <v>35931</v>
+        <v>35519</v>
       </c>
       <c r="O112" s="0" t="n">
         <v>6949</v>
@@ -8245,7 +8245,7 @@
         <v>37</v>
       </c>
       <c r="AA112" s="0" t="n">
-        <v>61617</v>
+        <v>27873</v>
       </c>
       <c r="AB112" s="0" t="n">
         <v>143106</v>
@@ -8254,13 +8254,13 @@
         <v>3005</v>
       </c>
       <c r="AD112" s="0" t="n">
-        <v>42259</v>
+        <v>39624</v>
       </c>
       <c r="AE112" s="0" t="n">
-        <v>19296</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16815</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="n">
         <v>2012</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>45671</v>
       </c>
       <c r="J113" s="0" t="n">
-        <v>111260</v>
+        <v>91936</v>
       </c>
       <c r="K113" s="0" t="n">
         <v>583320</v>
@@ -8301,7 +8301,7 @@
         <v>74010</v>
       </c>
       <c r="N113" s="0" t="n">
-        <v>37063</v>
+        <v>36679</v>
       </c>
       <c r="O113" s="0" t="n">
         <v>6950</v>
@@ -8340,7 +8340,7 @@
         <v>19</v>
       </c>
       <c r="AA113" s="0" t="n">
-        <v>64330</v>
+        <v>29127</v>
       </c>
       <c r="AB113" s="0" t="n">
         <v>143656</v>
@@ -8349,13 +8349,13 @@
         <v>2900</v>
       </c>
       <c r="AD113" s="0" t="n">
-        <v>43477</v>
+        <v>40685</v>
       </c>
       <c r="AE113" s="0" t="n">
-        <v>19933</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17322</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="n">
         <v>2013</v>
       </c>
@@ -8384,7 +8384,7 @@
         <v>47151</v>
       </c>
       <c r="J114" s="0" t="n">
-        <v>115921</v>
+        <v>95719</v>
       </c>
       <c r="K114" s="0" t="n">
         <v>585536</v>
@@ -8396,7 +8396,7 @@
         <v>75663</v>
       </c>
       <c r="N114" s="0" t="n">
-        <v>36000</v>
+        <v>35650</v>
       </c>
       <c r="O114" s="0" t="n">
         <v>6690</v>
@@ -8408,7 +8408,7 @@
         <v>36513</v>
       </c>
       <c r="R114" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S114" s="0" t="n">
         <v>0</v>
@@ -8435,7 +8435,7 @@
         <v>29</v>
       </c>
       <c r="AA114" s="0" t="n">
-        <v>68042</v>
+        <v>30789</v>
       </c>
       <c r="AB114" s="0" t="n">
         <v>149392</v>
@@ -8444,13 +8444,13 @@
         <v>2995</v>
       </c>
       <c r="AD114" s="0" t="n">
-        <v>44197</v>
+        <v>41246</v>
       </c>
       <c r="AE114" s="0" t="n">
-        <v>19481</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16701</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="n">
         <v>2014</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>48179</v>
       </c>
       <c r="J115" s="0" t="n">
-        <v>122002</v>
+        <v>101169</v>
       </c>
       <c r="K115" s="0" t="n">
         <v>592466</v>
@@ -8491,7 +8491,7 @@
         <v>76590</v>
       </c>
       <c r="N115" s="0" t="n">
-        <v>36055</v>
+        <v>35688</v>
       </c>
       <c r="O115" s="0" t="n">
         <v>6363</v>
@@ -8530,7 +8530,7 @@
         <v>23</v>
       </c>
       <c r="AA115" s="0" t="n">
-        <v>69087</v>
+        <v>30233</v>
       </c>
       <c r="AB115" s="0" t="n">
         <v>147299</v>
@@ -8539,13 +8539,13 @@
         <v>3045</v>
       </c>
       <c r="AD115" s="0" t="n">
-        <v>45451</v>
+        <v>42877</v>
       </c>
       <c r="AE115" s="0" t="n">
-        <v>18799</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16407</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="n">
         <v>2015</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>50016</v>
       </c>
       <c r="J116" s="0" t="n">
-        <v>132039</v>
+        <v>109441</v>
       </c>
       <c r="K116" s="0" t="n">
         <v>596730</v>
@@ -8586,7 +8586,7 @@
         <v>79622</v>
       </c>
       <c r="N116" s="0" t="n">
-        <v>38514</v>
+        <v>38093</v>
       </c>
       <c r="O116" s="0" t="n">
         <v>6095</v>
@@ -8598,7 +8598,7 @@
         <v>40428</v>
       </c>
       <c r="R116" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S116" s="0" t="n">
         <v>0</v>
@@ -8625,7 +8625,7 @@
         <v>19</v>
       </c>
       <c r="AA116" s="0" t="n">
-        <v>74078</v>
+        <v>32234</v>
       </c>
       <c r="AB116" s="0" t="n">
         <v>155305</v>
@@ -8634,13 +8634,13 @@
         <v>3067</v>
       </c>
       <c r="AD116" s="0" t="n">
-        <v>46999</v>
+        <v>44324</v>
       </c>
       <c r="AE116" s="0" t="n">
-        <v>20869</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18415</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="n">
         <v>2016</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>50090</v>
       </c>
       <c r="J117" s="0" t="n">
-        <v>145216</v>
+        <v>121768</v>
       </c>
       <c r="K117" s="0" t="n">
         <v>598817</v>
@@ -8681,7 +8681,7 @@
         <v>80144</v>
       </c>
       <c r="N117" s="0" t="n">
-        <v>41070</v>
+        <v>40651</v>
       </c>
       <c r="O117" s="0" t="n">
         <v>5737</v>
@@ -8720,7 +8720,7 @@
         <v>31</v>
       </c>
       <c r="AA117" s="0" t="n">
-        <v>77165</v>
+        <v>33267</v>
       </c>
       <c r="AB117" s="0" t="n">
         <v>154861</v>
@@ -8729,13 +8729,13 @@
         <v>3215</v>
       </c>
       <c r="AD117" s="0" t="n">
-        <v>48051</v>
+        <v>45076</v>
       </c>
       <c r="AE117" s="0" t="n">
-        <v>22798</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19994</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="n">
         <v>2017</v>
       </c>
@@ -8764,7 +8764,7 @@
         <v>50693</v>
       </c>
       <c r="J118" s="0" t="n">
-        <v>153526</v>
+        <v>130570</v>
       </c>
       <c r="K118" s="0" t="n">
         <v>600032</v>
@@ -8776,7 +8776,7 @@
         <v>83711</v>
       </c>
       <c r="N118" s="0" t="n">
-        <v>40971</v>
+        <v>40537</v>
       </c>
       <c r="O118" s="0" t="n">
         <v>5550</v>
@@ -8815,7 +8815,7 @@
         <v>31</v>
       </c>
       <c r="AA118" s="0" t="n">
-        <v>83087</v>
+        <v>35345</v>
       </c>
       <c r="AB118" s="0" t="n">
         <v>160498</v>
@@ -8824,10 +8824,10 @@
         <v>3359</v>
       </c>
       <c r="AD118" s="0" t="n">
-        <v>50409</v>
+        <v>47353</v>
       </c>
       <c r="AE118" s="0" t="n">
-        <v>23107</v>
+        <v>20225</v>
       </c>
     </row>
   </sheetData>
@@ -8848,8 +8848,8 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9952,7 +9952,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -10030,7 +10030,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>